<commit_message>
Corrected many tasks in in2010402
</commit_message>
<xml_diff>
--- a/in2010402/27-A.xlsx
+++ b/in2010402/27-A.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="27-A" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -838,15 +838,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D40"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>25</v>
       </c>
@@ -858,8 +858,19 @@
         <f>A1+A2+A9</f>
         <v>327</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F1">
+        <v>951</v>
+      </c>
+      <c r="G1">
+        <f>MOD(F1,3)</f>
+        <v>0</v>
+      </c>
+      <c r="I1">
+        <f>F1+F2+F15</f>
+        <v>2487</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>56</v>
       </c>
@@ -871,8 +882,19 @@
         <f>A1+A3+A4</f>
         <v>354</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>919</v>
+      </c>
+      <c r="G2">
+        <f t="shared" ref="G2:G40" si="1">MOD(F2,3)</f>
+        <v>1</v>
+      </c>
+      <c r="I2">
+        <f>F2+F3+F5</f>
+        <v>2697</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>136</v>
       </c>
@@ -884,8 +906,19 @@
         <f>A2+A5+A6</f>
         <v>465</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>898</v>
+      </c>
+      <c r="G3">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="I3">
+        <f>F1+F4+F18</f>
+        <v>2361</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>193</v>
       </c>
@@ -893,8 +926,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>894</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>203</v>
       </c>
@@ -902,8 +942,15 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>880</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>206</v>
       </c>
@@ -911,8 +958,15 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>874</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>215</v>
       </c>
@@ -920,8 +974,15 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>850</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>217</v>
       </c>
@@ -929,8 +990,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>838</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>246</v>
       </c>
@@ -938,8 +1006,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>832</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>268</v>
       </c>
@@ -947,8 +1022,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>775</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>273</v>
       </c>
@@ -956,8 +1038,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <v>724</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>286</v>
       </c>
@@ -965,8 +1054,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <v>694</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>308</v>
       </c>
@@ -974,8 +1070,15 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <v>691</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>323</v>
       </c>
@@ -983,8 +1086,15 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <v>667</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>364</v>
       </c>
@@ -992,8 +1102,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <v>617</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>375</v>
       </c>
@@ -1001,8 +1118,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>566</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>376</v>
       </c>
@@ -1010,8 +1134,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>523</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>406</v>
       </c>
@@ -1019,8 +1150,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <v>516</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>432</v>
       </c>
@@ -1028,8 +1166,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <v>513</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>487</v>
       </c>
@@ -1037,8 +1182,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <v>503</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>503</v>
       </c>
@@ -1046,8 +1198,15 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <v>487</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>513</v>
       </c>
@@ -1055,8 +1214,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <v>432</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>516</v>
       </c>
@@ -1064,8 +1230,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <v>406</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>523</v>
       </c>
@@ -1073,8 +1246,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <v>376</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>566</v>
       </c>
@@ -1082,8 +1262,15 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <v>375</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>617</v>
       </c>
@@ -1091,8 +1278,15 @@
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F26">
+        <v>364</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>667</v>
       </c>
@@ -1100,8 +1294,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F27">
+        <v>323</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>691</v>
       </c>
@@ -1109,8 +1310,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F28">
+        <v>308</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>694</v>
       </c>
@@ -1118,8 +1326,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F29">
+        <v>286</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>724</v>
       </c>
@@ -1127,8 +1342,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F30">
+        <v>273</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>775</v>
       </c>
@@ -1136,8 +1358,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F31">
+        <v>268</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>832</v>
       </c>
@@ -1145,8 +1374,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F32">
+        <v>246</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>838</v>
       </c>
@@ -1154,8 +1390,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F33">
+        <v>217</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>850</v>
       </c>
@@ -1163,8 +1406,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F34">
+        <v>215</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>874</v>
       </c>
@@ -1172,8 +1422,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F35">
+        <v>206</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>880</v>
       </c>
@@ -1181,8 +1438,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F36">
+        <v>203</v>
+      </c>
+      <c r="G36">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>894</v>
       </c>
@@ -1190,8 +1454,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F37">
+        <v>193</v>
+      </c>
+      <c r="G37">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>898</v>
       </c>
@@ -1199,8 +1470,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F38">
+        <v>136</v>
+      </c>
+      <c r="G38">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>919</v>
       </c>
@@ -1208,8 +1486,15 @@
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F39">
+        <v>56</v>
+      </c>
+      <c r="G39">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>951</v>
       </c>
@@ -1217,10 +1502,17 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
+      <c r="F40">
+        <v>25</v>
+      </c>
+      <c r="G40">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
-  <sortState ref="A1:A41">
-    <sortCondition ref="A1"/>
+  <sortState ref="F1:F40">
+    <sortCondition descending="1" ref="F1"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>